<commit_message>
reunion de scrum 6 y organizacion de plan de sprint
</commit_message>
<xml_diff>
--- a/Sprint2/Pila de sprint 2.xlsx
+++ b/Sprint2/Pila de sprint 2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Dropbox\EscenariosDeportivos\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Dropbox\EscenariosDeportivos\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B003BFF1-C55C-4AE6-A4DE-11641401E423}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -221,30 +220,18 @@
     <t>Atrasado</t>
   </si>
   <si>
-    <t xml:space="preserve">elaboracion de formularios de consulta </t>
-  </si>
-  <si>
     <t>Hector Mesa</t>
   </si>
   <si>
     <t>Mockup formularios</t>
   </si>
   <si>
-    <t>formularios de entrada y visualizacion de datos</t>
-  </si>
-  <si>
     <t>Implementacion</t>
   </si>
   <si>
-    <t>elaboracion de formularios de reserva</t>
-  </si>
-  <si>
     <t>Mockup de formularios</t>
   </si>
   <si>
-    <t>formularios de reservacion de escenarios</t>
-  </si>
-  <si>
     <t>modulo visual de administracion de escenarios</t>
   </si>
   <si>
@@ -417,12 +404,24 @@
   </si>
   <si>
     <t>Módulo de pagos en linea</t>
+  </si>
+  <si>
+    <t>formularios de pago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elaboracion de formularios de  pago </t>
+  </si>
+  <si>
+    <t>elaboracion de formularios para modificacion de reserva</t>
+  </si>
+  <si>
+    <t>formularios de modificacion de reserva</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -930,22 +929,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1329,11 +1328,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1344,10 +1343,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1399,7 +1398,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1455,66 +1454,66 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="54" t="s">
+      <c r="L6" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="55" t="s">
+      <c r="M6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="56" t="s">
+      <c r="N6" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
     </row>
     <row r="7" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="55"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="54"/>
       <c r="N7" s="8" t="s">
         <v>20</v>
       </c>
@@ -1564,7 +1563,7 @@
         <v>4</v>
       </c>
       <c r="M8" s="16">
-        <f t="shared" ref="M8:M22" si="0">L8-SUM(N8:Q8)</f>
+        <f t="shared" ref="M8:M23" si="0">L8-SUM(N8:Q8)</f>
         <v>4</v>
       </c>
       <c r="N8" s="17"/>
@@ -1638,7 +1637,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H10" s="31" t="s">
         <v>36</v>
@@ -1681,7 +1680,7 @@
         <v>29</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="30"/>
       <c r="H11" s="31" t="s">
@@ -1716,7 +1715,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D12" s="30">
         <v>1</v>
@@ -1729,7 +1728,7 @@
       </c>
       <c r="G12" s="30"/>
       <c r="H12" s="31" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I12" s="34">
         <v>43638</v>
@@ -2112,7 +2111,7 @@
         <v>59</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="30">
@@ -2154,36 +2153,36 @@
         <v>59</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30">
         <v>5</v>
       </c>
       <c r="F22" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="30" t="s">
-        <v>65</v>
-      </c>
       <c r="H22" s="31" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="I22" s="34">
-        <v>43613</v>
+        <v>43643</v>
       </c>
       <c r="J22" s="34">
-        <v>43614</v>
+        <v>43643</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>49</v>
       </c>
       <c r="L22" s="23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M22" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N22" s="32"/>
       <c r="O22" s="23"/>
@@ -2195,10 +2194,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="30">
@@ -2209,7 +2208,7 @@
       </c>
       <c r="G23" s="30"/>
       <c r="H23" s="31" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I23" s="35">
         <v>43643</v>
@@ -2223,13 +2222,16 @@
       <c r="L23" s="23">
         <v>2</v>
       </c>
-      <c r="M23" s="16"/>
+      <c r="M23" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="N23" s="32"/>
       <c r="O23" s="23"/>
       <c r="P23" s="23"/>
       <c r="Q23" s="24"/>
     </row>
-    <row r="24" spans="1:17" ht="57" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>17</v>
       </c>
@@ -2237,26 +2239,26 @@
         <v>59</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="30">
         <v>5</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="I24" s="35">
-        <v>43613</v>
+        <v>43643</v>
       </c>
       <c r="J24" s="35">
-        <v>43613</v>
+        <v>43643</v>
       </c>
       <c r="K24" s="15" t="s">
         <v>49</v>
@@ -2281,20 +2283,20 @@
         <v>59</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30">
         <v>5</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H25" s="31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I25" s="35">
         <v>43614</v>
@@ -2325,20 +2327,20 @@
         <v>59</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30">
         <v>4</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I26" s="35">
         <v>43614</v>
@@ -2369,20 +2371,20 @@
         <v>59</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D27" s="41"/>
       <c r="E27" s="41">
         <v>5</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H27" s="42" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I27" s="35">
         <v>43615</v>
@@ -2410,10 +2412,10 @@
         <v>21</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30">
@@ -2423,10 +2425,10 @@
         <v>60</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I28" s="45">
         <v>43616</v>
@@ -2454,20 +2456,20 @@
         <v>59</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="30">
         <v>5</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I29" s="45">
         <v>43616</v>
@@ -2495,20 +2497,20 @@
         <v>59</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30">
         <v>5</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I30" s="45">
         <v>43616</v>
@@ -2540,13 +2542,13 @@
         <v>4</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I31" s="45">
         <v>43617</v>
@@ -2571,21 +2573,21 @@
         <v>25</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30">
         <v>4</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G32" s="30"/>
       <c r="H32" s="30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I32" s="45">
         <v>43645</v>
@@ -2613,20 +2615,20 @@
         <v>59</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="30">
         <v>3</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I33" s="45">
         <v>43616</v>
@@ -2651,21 +2653,21 @@
         <v>27</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="57" t="s">
-        <v>127</v>
+        <v>84</v>
+      </c>
+      <c r="C34" s="52" t="s">
+        <v>123</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30">
         <v>3</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G34" s="30"/>
-      <c r="H34" s="57" t="s">
-        <v>128</v>
+      <c r="H34" s="52" t="s">
+        <v>124</v>
       </c>
       <c r="I34" s="45">
         <v>43649</v>
@@ -2693,20 +2695,20 @@
         <v>59</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D35" s="47"/>
       <c r="E35" s="47">
         <v>3</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H35" s="23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I35" s="45">
         <v>43617</v>
@@ -2731,20 +2733,20 @@
         <v>29</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D36" s="47"/>
       <c r="E36" s="47">
         <v>3</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="48">
@@ -2791,21 +2793,21 @@
         <v>31</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D38" s="47"/>
       <c r="E38" s="47">
         <v>3</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G38" s="23"/>
       <c r="H38" s="23" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I38" s="48"/>
       <c r="J38" s="47"/>
@@ -2825,7 +2827,7 @@
       </c>
       <c r="B39" s="47"/>
       <c r="C39" s="47" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
@@ -2848,7 +2850,7 @@
       </c>
       <c r="B40" s="47"/>
       <c r="C40" s="47" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D40" s="47"/>
       <c r="E40" s="47"/>
@@ -2927,7 +2929,7 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="51" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>29</v>
@@ -2937,7 +2939,7 @@
       <c r="H44" s="39"/>
       <c r="I44" s="39"/>
       <c r="J44" s="51" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K44" s="7" t="s">
         <v>49</v>
@@ -2952,10 +2954,10 @@
     <row r="45" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
       <c r="B45" s="51" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="7" t="s">
@@ -2967,7 +2969,7 @@
       <c r="I45" s="39"/>
       <c r="J45" s="39"/>
       <c r="K45" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="L45" s="39"/>
       <c r="M45" s="39"/>
@@ -2980,11 +2982,11 @@
       <c r="A46" s="39"/>
       <c r="B46" s="39"/>
       <c r="C46" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F46" s="39"/>
       <c r="G46" s="39"/>
@@ -3005,11 +3007,11 @@
       <c r="A47" s="39"/>
       <c r="B47" s="39"/>
       <c r="C47" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F47" s="39"/>
       <c r="G47" s="39"/>
@@ -3034,7 +3036,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F48" s="39"/>
       <c r="G48" s="39"/>
@@ -3074,7 +3076,7 @@
       <c r="A50" s="39"/>
       <c r="B50" s="39"/>
       <c r="C50" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="39"/>
@@ -3116,7 +3118,7 @@
       <c r="A52" s="39"/>
       <c r="B52" s="39"/>
       <c r="C52" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="39"/>
@@ -3135,21 +3137,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Se modifica la pila
</commit_message>
<xml_diff>
--- a/Sprint2/Pila de sprint 2.xlsx
+++ b/Sprint2/Pila de sprint 2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>formularios de modificacion de reserva</t>
+  </si>
+  <si>
+    <t>terminado</t>
+  </si>
+  <si>
+    <t>Juan Sebastian Sanchez</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -470,6 +476,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -778,7 +791,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -932,6 +945,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -941,11 +960,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1331,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1343,10 +1359,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1379,7 +1395,7 @@
       <c r="E2" s="5">
         <v>43636</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="58"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1454,66 +1470,66 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="53" t="s">
+      <c r="K6" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="53" t="s">
+      <c r="L6" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="54" t="s">
+      <c r="M6" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="55" t="s">
+      <c r="N6" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
     </row>
     <row r="7" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="54"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="56"/>
       <c r="N7" s="8" t="s">
         <v>20</v>
       </c>
@@ -1557,14 +1573,14 @@
         <v>43636</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L8" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M8" s="16">
         <f t="shared" ref="M8:M23" si="0">L8-SUM(N8:Q8)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N8" s="17"/>
       <c r="O8" s="23"/>
@@ -1603,14 +1619,14 @@
         <v>43636</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L9" s="25">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="M9" s="16">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="N9" s="17"/>
       <c r="O9" s="28"/>
@@ -1649,14 +1665,14 @@
         <v>43637</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L10" s="23">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M10" s="16">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="23"/>
@@ -1693,7 +1709,7 @@
         <v>43641</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L11" s="23">
         <v>0.5</v>
@@ -1737,14 +1753,14 @@
         <v>43638</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L12" s="23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M12" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N12" s="32"/>
       <c r="O12" s="23"/>
@@ -1781,14 +1797,14 @@
         <v>43638</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L13" s="23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M13" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N13" s="32"/>
       <c r="O13" s="23"/>
@@ -1825,14 +1841,14 @@
         <v>43639</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L14" s="23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M14" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N14" s="32"/>
       <c r="O14" s="23"/>
@@ -1913,7 +1929,7 @@
         <v>43648</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L16" s="23">
         <v>1</v>
@@ -1944,7 +1960,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="G17" s="30"/>
       <c r="H17" s="31" t="s">
@@ -1957,7 +1973,7 @@
         <v>43639</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="L17" s="23">
         <v>5</v>
@@ -1988,7 +2004,7 @@
         <v>29</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="G18" s="30"/>
       <c r="H18" s="31" t="s">
@@ -2032,7 +2048,7 @@
         <v>29</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="G19" s="30"/>
       <c r="H19" s="31" t="s">
@@ -2076,7 +2092,7 @@
         <v>40</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="G20" s="30"/>
       <c r="H20" s="31" t="s">
@@ -3137,23 +3153,23 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:Q6"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reunión de sprint 7
</commit_message>
<xml_diff>
--- a/Sprint2/Pila de sprint 2.xlsx
+++ b/Sprint2/Pila de sprint 2.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Dropbox\EscenariosDeportivos\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\U\Laboratorio de software\EscenariosDeportivos\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0A0012-850D-482E-9751-540CDE1B359E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="120">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -232,33 +233,6 @@
     <t>Mockup de formularios</t>
   </si>
   <si>
-    <t>modulo visual de administracion de escenarios</t>
-  </si>
-  <si>
-    <t>Mockup de interfaz grafica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modulo grafico administrador de escenarios </t>
-  </si>
-  <si>
-    <t>Pantalla de inicio del sistema</t>
-  </si>
-  <si>
-    <t>Mockup de inicio del sistema</t>
-  </si>
-  <si>
-    <t>interfaz grafica de inicio del sistema</t>
-  </si>
-  <si>
-    <t>Mapa de escenarios deportivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Framework google maps </t>
-  </si>
-  <si>
-    <t>vinculacion grafica del framework de Google Maps</t>
-  </si>
-  <si>
     <t xml:space="preserve">interfaz grafica de actualizacion y mantenimiento </t>
   </si>
   <si>
@@ -275,12 +249,6 @@
   </si>
   <si>
     <t>Formularios con responsive Design</t>
-  </si>
-  <si>
-    <t>framework de pago, Mockup de formularios de pago</t>
-  </si>
-  <si>
-    <t>Formularios de medios de pago electronico</t>
   </si>
   <si>
     <t>Desarrollo</t>
@@ -427,7 +395,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -498,7 +466,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -682,32 +650,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -761,37 +703,13 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -844,7 +762,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -853,42 +780,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -913,18 +825,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -938,13 +838,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -959,9 +864,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1344,11 +1246,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1359,10 +1261,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="48"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +1297,7 @@
       <c r="E2" s="5">
         <v>43636</v>
       </c>
-      <c r="F2" s="58"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1414,7 +1316,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1470,66 +1372,66 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="55" t="s">
+      <c r="J6" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="55" t="s">
+      <c r="K6" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="55" t="s">
+      <c r="L6" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="56" t="s">
+      <c r="M6" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="57" t="s">
+      <c r="N6" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
     </row>
     <row r="7" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="56"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="51"/>
       <c r="N7" s="8" t="s">
         <v>20</v>
       </c>
@@ -1544,10 +1446,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
+      <c r="A8" s="18">
         <v>1</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -1563,7 +1465,7 @@
       <c r="G8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="20" t="s">
         <v>31</v>
       </c>
       <c r="I8" s="14">
@@ -1573,43 +1475,45 @@
         <v>43636</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L8" s="21">
+        <v>118</v>
+      </c>
+      <c r="L8" s="19">
         <v>1</v>
       </c>
       <c r="M8" s="16">
         <f t="shared" ref="M8:M23" si="0">L8-SUM(N8:Q8)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="17">
         <v>1</v>
       </c>
-      <c r="N8" s="17"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="24"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="22"/>
     </row>
     <row r="9" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>2</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="24">
         <v>1</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="25" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="14">
@@ -1619,31 +1523,33 @@
         <v>43636</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L9" s="25">
+        <v>118</v>
+      </c>
+      <c r="L9" s="23">
         <v>3</v>
       </c>
       <c r="M9" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="17">
         <v>3</v>
       </c>
-      <c r="N9" s="17"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="29"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="27"/>
     </row>
     <row r="10" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
+      <c r="A10" s="18">
         <v>3</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="28">
         <v>2</v>
       </c>
       <c r="E10" s="13" t="s">
@@ -1653,9 +1559,9 @@
         <v>5</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="H10" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="29" t="s">
         <v>36</v>
       </c>
       <c r="I10" s="14">
@@ -1665,31 +1571,33 @@
         <v>43637</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L10" s="23">
+        <v>118</v>
+      </c>
+      <c r="L10" s="21">
         <v>3</v>
       </c>
       <c r="M10" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="30">
         <v>3</v>
       </c>
-      <c r="N10" s="32"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="24"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="22"/>
     </row>
     <row r="11" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>4</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="28" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="13" t="s">
@@ -1698,42 +1606,44 @@
       <c r="F11" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31" t="s">
+      <c r="G11" s="28"/>
+      <c r="H11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="31">
         <v>43641</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="31">
         <v>43641</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L11" s="23">
+        <v>118</v>
+      </c>
+      <c r="L11" s="21">
         <v>0.5</v>
       </c>
       <c r="M11" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="30">
         <v>0.5</v>
       </c>
-      <c r="N11" s="32"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="24"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="22"/>
     </row>
     <row r="12" spans="1:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="A12" s="18">
         <v>5</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="30">
+      <c r="C12" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="28">
         <v>1</v>
       </c>
       <c r="E12" s="13" t="s">
@@ -1742,42 +1652,44 @@
       <c r="F12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="I12" s="34">
+      <c r="G12" s="28"/>
+      <c r="H12" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="32">
         <v>43638</v>
       </c>
-      <c r="J12" s="35">
+      <c r="J12" s="33">
         <v>43638</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L12" s="23">
+        <v>118</v>
+      </c>
+      <c r="L12" s="21">
         <v>1</v>
       </c>
       <c r="M12" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="30">
         <v>1</v>
       </c>
-      <c r="N12" s="32"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="24"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="22"/>
     </row>
     <row r="13" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>6</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="28">
         <v>1</v>
       </c>
       <c r="E13" s="13" t="s">
@@ -1786,42 +1698,44 @@
       <c r="F13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31" t="s">
+      <c r="G13" s="28"/>
+      <c r="H13" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="32">
         <v>43638</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="32">
         <v>43638</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L13" s="23">
+        <v>118</v>
+      </c>
+      <c r="L13" s="21">
         <v>1</v>
       </c>
       <c r="M13" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="30">
         <v>1</v>
       </c>
-      <c r="N13" s="32"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="24"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="22"/>
     </row>
     <row r="14" spans="1:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="A14" s="18">
         <v>7</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <v>1</v>
       </c>
       <c r="E14" s="13" t="s">
@@ -1830,30 +1744,32 @@
       <c r="F14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31" t="s">
+      <c r="G14" s="28"/>
+      <c r="H14" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="32">
         <v>43639</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="32">
         <v>43639</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L14" s="23">
+        <v>118</v>
+      </c>
+      <c r="L14" s="21">
         <v>3</v>
       </c>
       <c r="M14" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="30">
         <v>3</v>
       </c>
-      <c r="N14" s="32"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="24"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="22"/>
     </row>
     <row r="15" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
@@ -1869,16 +1785,16 @@
       <c r="E15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="36">
         <v>43640</v>
       </c>
       <c r="J15" s="5">
@@ -1887,1269 +1803,1109 @@
       <c r="K15" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L15" s="37">
+      <c r="L15" s="35">
         <v>3</v>
       </c>
       <c r="M15" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
     </row>
     <row r="16" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="20">
+      <c r="A16" s="18">
         <v>9</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31" t="s">
+      <c r="G16" s="28"/>
+      <c r="H16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="35">
+      <c r="I16" s="33">
         <v>43648</v>
       </c>
-      <c r="J16" s="35">
+      <c r="J16" s="33">
         <v>43648</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L16" s="23">
+        <v>118</v>
+      </c>
+      <c r="L16" s="21">
         <v>1</v>
       </c>
       <c r="M16" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="30">
         <v>1</v>
       </c>
-      <c r="N16" s="32"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="24"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="22"/>
     </row>
     <row r="17" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>10</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="28">
         <v>5</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31" t="s">
+      <c r="F17" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="33">
         <v>43639</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="33">
         <v>43639</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L17" s="23">
+        <v>118</v>
+      </c>
+      <c r="L17" s="21">
         <v>5</v>
       </c>
       <c r="M17" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N17" s="32"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="24"/>
+        <v>2</v>
+      </c>
+      <c r="N17" s="30">
+        <v>3</v>
+      </c>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="22"/>
     </row>
     <row r="18" spans="1:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="A18" s="20">
+      <c r="A18" s="18">
         <v>11</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="28">
         <v>10</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="31" t="s">
+      <c r="F18" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="28"/>
+      <c r="H18" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I18" s="33">
         <v>43640</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="33">
         <v>43640</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L18" s="23">
+        <v>118</v>
+      </c>
+      <c r="L18" s="21">
         <v>5</v>
       </c>
       <c r="M18" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N18" s="32"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="24"/>
+        <v>4</v>
+      </c>
+      <c r="N18" s="30">
+        <v>1</v>
+      </c>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="22"/>
     </row>
     <row r="19" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>12</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="28">
         <v>11</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31" t="s">
+      <c r="F19" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="I19" s="35">
+      <c r="I19" s="33">
         <v>43640</v>
       </c>
-      <c r="J19" s="35">
+      <c r="J19" s="33">
         <v>43640</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L19" s="23">
+        <v>118</v>
+      </c>
+      <c r="L19" s="21">
         <v>5</v>
       </c>
       <c r="M19" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N19" s="32"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="24"/>
+        <v>2</v>
+      </c>
+      <c r="N19" s="30">
+        <v>3</v>
+      </c>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="22"/>
     </row>
     <row r="20" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="20">
+      <c r="A20" s="18">
         <v>13</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="28">
         <v>12</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31" t="s">
+      <c r="F20" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I20" s="33">
         <v>43641</v>
       </c>
-      <c r="J20" s="35">
+      <c r="J20" s="33">
         <v>43641</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L20" s="23">
+        <v>118</v>
+      </c>
+      <c r="L20" s="21">
         <v>3</v>
       </c>
       <c r="M20" s="16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="30">
         <v>3</v>
       </c>
-      <c r="N20" s="32"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="24"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="22"/>
     </row>
     <row r="21" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>14</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30">
+      <c r="C21" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28">
         <v>5</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="31" t="s">
+      <c r="G21" s="28"/>
+      <c r="H21" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="33">
         <v>43642</v>
       </c>
-      <c r="J21" s="35">
+      <c r="J21" s="33">
         <v>43642</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L21" s="21">
         <v>10</v>
       </c>
       <c r="M21" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N21" s="32"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="24"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="22"/>
     </row>
     <row r="22" spans="1:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="A22" s="20">
+      <c r="A22" s="18">
         <v>15</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30">
+      <c r="C22" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28">
         <v>5</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="I22" s="34">
+      <c r="H22" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="32">
         <v>43643</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="32">
         <v>43643</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="21">
         <v>2</v>
       </c>
       <c r="M22" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="N22" s="32"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="24"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="22"/>
     </row>
     <row r="23" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>16</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30">
+      <c r="C23" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28">
         <v>5</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="I23" s="35">
+      <c r="G23" s="28"/>
+      <c r="H23" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="33">
         <v>43643</v>
       </c>
-      <c r="J23" s="35">
+      <c r="J23" s="33">
         <v>43643</v>
       </c>
       <c r="K23" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L23" s="23">
+      <c r="L23" s="21">
         <v>2</v>
       </c>
       <c r="M23" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="N23" s="32"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="24"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="22"/>
     </row>
     <row r="24" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="20">
+      <c r="A24" s="18">
         <v>17</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30">
+      <c r="C24" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28">
         <v>5</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H24" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="I24" s="35">
+      <c r="H24" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="33">
         <v>43643</v>
       </c>
-      <c r="J24" s="35">
+      <c r="J24" s="33">
         <v>43643</v>
       </c>
       <c r="K24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="21">
         <v>2</v>
       </c>
       <c r="M24" s="16">
         <f>L24-SUM(N24:Q24)</f>
         <v>2</v>
       </c>
-      <c r="N24" s="32"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="24"/>
-    </row>
-    <row r="25" spans="1:17" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
-        <v>18</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30">
-        <v>5</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" s="35">
-        <v>43614</v>
-      </c>
-      <c r="J25" s="35">
-        <v>43614</v>
+      <c r="N24" s="30"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="22"/>
+    </row>
+    <row r="25" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
+        <v>21</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28">
+        <v>4</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="39">
+        <v>43616</v>
+      </c>
+      <c r="J25" s="39">
+        <v>43616</v>
       </c>
       <c r="K25" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="23">
+      <c r="L25" s="21">
+        <v>3</v>
+      </c>
+      <c r="M25" s="40"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+    </row>
+    <row r="26" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>22</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28">
         <v>5</v>
       </c>
-      <c r="M25" s="16">
-        <f>L25-SUM(N25:Q25)</f>
-        <v>5</v>
-      </c>
-      <c r="N25" s="32"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="24"/>
-    </row>
-    <row r="26" spans="1:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="A26" s="20">
-        <v>19</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30">
-        <v>4</v>
-      </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="H26" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" s="35">
-        <v>43614</v>
-      </c>
-      <c r="J26" s="35">
-        <v>43615</v>
+      <c r="G26" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" s="39">
+        <v>43643</v>
+      </c>
+      <c r="J26" s="39">
+        <v>43643</v>
       </c>
       <c r="K26" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="23">
-        <v>2</v>
-      </c>
-      <c r="M26" s="16">
-        <f>L26-SUM(N26:Q26)</f>
-        <v>2</v>
-      </c>
-      <c r="N26" s="32"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="24"/>
-    </row>
-    <row r="27" spans="1:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="A27" s="11">
-        <v>20</v>
-      </c>
-      <c r="B27" s="41" t="s">
+      <c r="L26" s="21">
+        <v>5</v>
+      </c>
+      <c r="M26" s="40"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+    </row>
+    <row r="27" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="18">
+        <v>23</v>
+      </c>
+      <c r="B27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41">
+      <c r="C27" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28">
         <v>5</v>
       </c>
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="H27" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="I27" s="35">
-        <v>43615</v>
-      </c>
-      <c r="J27" s="43">
-        <v>43615</v>
+      <c r="G27" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="39">
+        <v>43644</v>
+      </c>
+      <c r="J27" s="39">
+        <v>43644</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="21">
         <v>2</v>
       </c>
-      <c r="M27" s="16">
-        <f>L27-SUM(N27:Q27)</f>
-        <v>2</v>
-      </c>
-      <c r="N27" s="44"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="19"/>
-    </row>
-    <row r="28" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="20">
-        <v>21</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30">
+      <c r="M27" s="40"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+    </row>
+    <row r="28" spans="1:17" ht="57" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
+        <v>25</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28">
         <v>4</v>
       </c>
-      <c r="F28" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="I28" s="45">
-        <v>43616</v>
-      </c>
-      <c r="J28" s="45">
-        <v>43616</v>
+      <c r="F28" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="39">
+        <v>43645</v>
+      </c>
+      <c r="J28" s="39">
+        <v>43649</v>
       </c>
       <c r="K28" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L28" s="23">
+      <c r="L28" s="21">
+        <v>5</v>
+      </c>
+      <c r="M28" s="40"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+    </row>
+    <row r="29" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
+        <v>26</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28">
         <v>3</v>
       </c>
-      <c r="M28" s="46"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-    </row>
-    <row r="29" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="11">
-        <v>22</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="30" t="s">
+      <c r="F29" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30">
-        <v>5</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" s="30" t="s">
+      <c r="H29" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" s="45">
-        <v>43616</v>
-      </c>
-      <c r="J29" s="45">
-        <v>43616</v>
+      <c r="I29" s="39">
+        <v>43645</v>
+      </c>
+      <c r="J29" s="39">
+        <v>43645</v>
       </c>
       <c r="K29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L29" s="23">
-        <v>5</v>
-      </c>
-      <c r="M29" s="46"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-    </row>
-    <row r="30" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="20">
-        <v>23</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30">
-        <v>5</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="I30" s="45">
-        <v>43616</v>
-      </c>
-      <c r="J30" s="45">
-        <v>43616</v>
+      <c r="L29" s="21">
+        <v>2</v>
+      </c>
+      <c r="M29" s="40"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+    </row>
+    <row r="30" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="18">
+        <v>27</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28">
+        <v>3</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="39">
+        <v>43649</v>
+      </c>
+      <c r="J30" s="39">
+        <v>43651</v>
       </c>
       <c r="K30" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L30" s="23">
-        <v>2</v>
-      </c>
-      <c r="M30" s="46"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-    </row>
-    <row r="31" spans="1:17" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="L30" s="21">
+        <v>10</v>
+      </c>
+      <c r="M30" s="40"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+    </row>
+    <row r="31" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
-        <v>24</v>
-      </c>
-      <c r="B31" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30">
-        <v>4</v>
-      </c>
-      <c r="F31" s="30" t="s">
+      <c r="C31" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41">
+        <v>3</v>
+      </c>
+      <c r="F31" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G31" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="I31" s="45">
-        <v>43617</v>
-      </c>
-      <c r="J31" s="45">
-        <v>43617</v>
+      <c r="G31" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="39">
+        <v>43645</v>
+      </c>
+      <c r="J31" s="39">
+        <v>43645</v>
       </c>
       <c r="K31" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L31" s="23">
+      <c r="L31" s="21">
+        <v>2</v>
+      </c>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+    </row>
+    <row r="32" spans="1:17" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="18">
+        <v>29</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41">
         <v>3</v>
       </c>
-      <c r="M31" s="46"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-    </row>
-    <row r="32" spans="1:17" ht="57" x14ac:dyDescent="0.2">
-      <c r="A32" s="20">
-        <v>25</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30">
-        <v>4</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="I32" s="45">
-        <v>43645</v>
-      </c>
-      <c r="J32" s="45">
-        <v>43649</v>
+      <c r="F32" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="21"/>
+      <c r="I32" s="42">
+        <v>43619</v>
+      </c>
+      <c r="J32" s="42">
+        <v>43619</v>
       </c>
       <c r="K32" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L32" s="23">
-        <v>5</v>
-      </c>
-      <c r="M32" s="46"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-    </row>
-    <row r="33" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="L32" s="21">
+        <v>2</v>
+      </c>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+    </row>
+    <row r="33" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
-        <v>26</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30">
+        <v>30</v>
+      </c>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+    </row>
+    <row r="34" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="18">
+        <v>31</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41">
         <v>3</v>
       </c>
-      <c r="F33" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="H33" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="I33" s="45">
-        <v>43616</v>
-      </c>
-      <c r="J33" s="45">
-        <v>43616</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L33" s="23">
-        <v>2</v>
-      </c>
-      <c r="M33" s="46"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="23"/>
-    </row>
-    <row r="34" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="20">
-        <v>27</v>
-      </c>
-      <c r="B34" s="30" t="s">
+      <c r="F34" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30">
-        <v>3</v>
-      </c>
-      <c r="F34" s="30" t="s">
+      <c r="G34" s="21"/>
+      <c r="H34" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="G34" s="30"/>
-      <c r="H34" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="I34" s="45">
-        <v>43649</v>
-      </c>
-      <c r="J34" s="45">
-        <v>43651</v>
-      </c>
+      <c r="I34" s="42"/>
+      <c r="J34" s="41"/>
       <c r="K34" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="23">
-        <v>10</v>
-      </c>
-      <c r="M34" s="46"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="23"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
     </row>
     <row r="35" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
-        <v>28</v>
-      </c>
-      <c r="B35" s="47" t="s">
-        <v>59</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B35" s="41"/>
       <c r="C35" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+    </row>
+    <row r="36" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="18">
+        <v>33</v>
+      </c>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+    </row>
+    <row r="37" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="37"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+    </row>
+    <row r="38" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="37"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
+    </row>
+    <row r="39" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="37"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+    </row>
+    <row r="40" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="37"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47">
-        <v>3</v>
-      </c>
-      <c r="F35" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G35" s="30" t="s">
+      <c r="K40" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="37"/>
+      <c r="O40" s="37"/>
+      <c r="P40" s="37"/>
+      <c r="Q40" s="37"/>
+    </row>
+    <row r="41" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A41" s="37"/>
+      <c r="B41" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="C41" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I35" s="45">
-        <v>43617</v>
-      </c>
-      <c r="J35" s="45">
-        <v>43617</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L35" s="23">
-        <v>2</v>
-      </c>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23"/>
-      <c r="Q35" s="23"/>
-    </row>
-    <row r="36" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="20">
-        <v>29</v>
-      </c>
-      <c r="B36" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="47" t="s">
+      <c r="D41" s="2"/>
+      <c r="E41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47">
-        <v>3</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G36" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="H36" s="23"/>
-      <c r="I36" s="48">
-        <v>43619</v>
-      </c>
-      <c r="J36" s="48">
-        <v>43619</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L36" s="23">
-        <v>2</v>
-      </c>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="23"/>
-    </row>
-    <row r="37" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="11">
-        <v>30</v>
-      </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="49"/>
-    </row>
-    <row r="38" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="20">
-        <v>31</v>
-      </c>
-      <c r="B38" s="47" t="s">
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="37"/>
+      <c r="O41" s="37"/>
+      <c r="P41" s="37"/>
+      <c r="Q41" s="37"/>
+    </row>
+    <row r="42" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="D42" s="2"/>
+      <c r="E42" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47">
-        <v>3</v>
-      </c>
-      <c r="F38" s="23" t="s">
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
+      <c r="O42" s="37"/>
+      <c r="P42" s="37"/>
+      <c r="Q42" s="37"/>
+    </row>
+    <row r="43" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23" t="s">
+      <c r="D43" s="2"/>
+      <c r="E43" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I38" s="48"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="23"/>
-      <c r="Q38" s="23"/>
-    </row>
-    <row r="39" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="11">
-        <v>32</v>
-      </c>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47" t="s">
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L43" s="37"/>
+      <c r="M43" s="37"/>
+      <c r="N43" s="37"/>
+      <c r="O43" s="37"/>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+    </row>
+    <row r="44" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
-    </row>
-    <row r="40" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="20">
-        <v>33</v>
-      </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47" t="s">
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
+      <c r="O44" s="37"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+    </row>
+    <row r="45" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+    </row>
+    <row r="46" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="23"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
-    </row>
-    <row r="41" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="39"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
-      <c r="O41" s="39"/>
-      <c r="P41" s="39"/>
-      <c r="Q41" s="39"/>
-    </row>
-    <row r="42" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
-      <c r="Q42" s="39"/>
-    </row>
-    <row r="43" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="51"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="39"/>
-      <c r="P43" s="39"/>
-      <c r="Q43" s="39"/>
-    </row>
-    <row r="44" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="39"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="51" t="s">
+      <c r="D46" s="2"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="37"/>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="37"/>
+    </row>
+    <row r="47" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+    </row>
+    <row r="48" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
-      <c r="Q44" s="39"/>
-    </row>
-    <row r="45" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
-      <c r="O45" s="39"/>
-      <c r="P45" s="39"/>
-      <c r="Q45" s="39"/>
-    </row>
-    <row r="46" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="39"/>
-      <c r="P46" s="39"/>
-      <c r="Q46" s="39"/>
-    </row>
-    <row r="47" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="K47" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L47" s="39"/>
-      <c r="M47" s="39"/>
-      <c r="N47" s="39"/>
-      <c r="O47" s="39"/>
-      <c r="P47" s="39"/>
-      <c r="Q47" s="39"/>
-    </row>
-    <row r="48" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
-      <c r="M48" s="39"/>
-      <c r="N48" s="39"/>
-      <c r="O48" s="39"/>
-      <c r="P48" s="39"/>
-      <c r="Q48" s="39"/>
-    </row>
-    <row r="49" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="39"/>
-      <c r="N49" s="39"/>
-      <c r="O49" s="39"/>
-      <c r="P49" s="39"/>
-      <c r="Q49" s="39"/>
-    </row>
-    <row r="50" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
-      <c r="O50" s="39"/>
-      <c r="P50" s="39"/>
-      <c r="Q50" s="39"/>
-    </row>
-    <row r="51" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="39"/>
-      <c r="N51" s="39"/>
-      <c r="O51" s="39"/>
-      <c r="P51" s="39"/>
-      <c r="Q51" s="39"/>
-    </row>
-    <row r="52" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="39"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="39"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="39"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>